<commit_message>
Updated BOM. Added time estimate.
</commit_message>
<xml_diff>
--- a/SwitchPanel/BOM.xlsx
+++ b/SwitchPanel/BOM.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="15990"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Switch Panel Parts</t>
   </si>
@@ -58,72 +61,150 @@
   </si>
   <si>
     <t>Wire - 25ft Spool</t>
+  </si>
+  <si>
+    <t>Power Cable Connector</t>
+  </si>
+  <si>
+    <t>Solenoid Lock</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>Adafruit Trinket 5V</t>
   </si>
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>http://www.amazon.com/dp/B003N3DQOI/ref=wl_it_dp_o_pC_S_ttl?_encoding=UTF8&amp;colid=3JVFEFB4A7MPJ&amp;coliid=I1NN6OC4KDZV5M</t>
     </r>
   </si>
   <si>
-    <t>12V Power Supply</t>
-  </si>
-  <si>
-    <t>Power Cable</t>
-  </si>
-  <si>
-    <t>Power Cable Connector</t>
-  </si>
-  <si>
-    <t>Solenoid Lock</t>
-  </si>
-  <si>
-    <t>Adafruit</t>
-  </si>
-  <si>
-    <t>Adafruit Trinket 5V</t>
-  </si>
-  <si>
-    <t>5V Voltage Regulator</t>
+    <t>Diode - 1N4001</t>
+  </si>
+  <si>
+    <r>
+      <t>Resistor - 2.2k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+  </si>
+  <si>
+    <t>Darlington Transistor - TIP120</t>
+  </si>
+  <si>
+    <t>Perma Proto Half Size Breadboard</t>
+  </si>
+  <si>
+    <t>12V 1A Power Supply</t>
+  </si>
+  <si>
+    <t>http://www.amazon.com/uxcell-Switching-Power-Supply-Driver/dp/B00CQFUZFC/ref=sr_1_12?ie=UTF8&amp;qid=1461683926&amp;sr=8-12&amp;keywords=12V+2A+Power+supply</t>
+  </si>
+  <si>
+    <t>Power Cable - 7.5ft</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total +</t>
+  </si>
+  <si>
+    <t>Adafruit JST Breakout</t>
+  </si>
+  <si>
+    <t>Design Circuit</t>
+  </si>
+  <si>
+    <t>Design Panel</t>
+  </si>
+  <si>
+    <t>Cut Panel</t>
+  </si>
+  <si>
+    <t>Mount Switches</t>
+  </si>
+  <si>
+    <t>Crimp connectors</t>
+  </si>
+  <si>
+    <t>Solder PCB</t>
+  </si>
+  <si>
+    <t>Program Trinket</t>
+  </si>
+  <si>
+    <t>Test Trinket</t>
+  </si>
+  <si>
+    <t>Test Whole Panel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* (#,##0.00);&quot; &quot;&quot;$&quot;* &quot;-&quot;??&quot; &quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* \(#,##0.00\);&quot; &quot;&quot;$&quot;* &quot;-&quot;??&quot; &quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Helvetica"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color indexed="8"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <u val="single"/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color indexed="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,8 +217,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -160,73 +247,411 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="10"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="10"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="10"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="47">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -352,7 +777,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -361,7 +786,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -370,7 +795,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -444,7 +869,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -452,7 +877,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -471,7 +896,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -501,7 +926,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -527,7 +952,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -553,7 +978,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -579,7 +1004,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -605,7 +1030,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -631,7 +1056,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -657,7 +1082,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -683,7 +1108,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -709,7 +1134,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -722,9 +1147,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -739,7 +1170,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -747,7 +1178,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -766,7 +1197,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -792,7 +1223,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -818,7 +1249,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -844,7 +1275,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -870,7 +1301,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -896,7 +1327,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -922,7 +1353,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -948,7 +1379,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -974,7 +1405,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1000,7 +1431,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1013,9 +1444,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1029,7 +1466,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1048,7 +1485,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1078,7 +1515,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1104,7 +1541,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1130,7 +1567,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1156,7 +1593,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1182,7 +1619,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1208,7 +1645,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1234,7 +1671,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1260,7 +1697,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1286,7 +1723,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1299,247 +1736,440 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85156" style="1" customWidth="1"/>
-    <col min="7" max="256" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="4" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="2">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="D2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="E2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="2">
+      <c r="F2" s="36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="2">
+    <row r="3" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="31">
         <v>70192226</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="31">
         <v>12</v>
       </c>
-      <c r="E3" s="5">
-        <v>4.23</v>
-      </c>
-      <c r="F3" s="6">
-        <f>E3*D3</f>
-        <v>50.76000000000001</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="2">
+      <c r="E3" s="32">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="F3" s="33">
+        <f t="shared" ref="F3:F18" si="0">E3*D3</f>
+        <v>50.760000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4">
+      <c r="C4" s="14"/>
+      <c r="D4" s="11">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="15">
         <v>5</v>
       </c>
-      <c r="F4" s="6">
-        <f>E4*D4</f>
+      <c r="F4" s="13">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="2">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s" s="7">
+      <c r="C5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="11">
         <v>1</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="12">
         <v>6.99</v>
       </c>
-      <c r="F5" s="6">
-        <f>E5*D5</f>
+      <c r="F5" s="13">
+        <f t="shared" si="0"/>
         <v>6.99</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="2">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="B6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s" s="7">
+      <c r="C6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1</v>
+      </c>
+      <c r="E6" s="15">
+        <v>6.4</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="0"/>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
+      <c r="E7" s="15">
+        <v>7.7</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="0"/>
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="14">
+        <v>70115988</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15">
+        <v>2.93</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="0"/>
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="4">
+      <c r="B9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="14">
+        <v>70133360</v>
+      </c>
+      <c r="D9" s="11">
         <v>1</v>
       </c>
-      <c r="E6" s="6">
-        <v>6.4</v>
-      </c>
-      <c r="F6" s="6">
-        <f>E6*D6</f>
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="2">
+      <c r="E9" s="15">
+        <v>0.54</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4">
+      <c r="B10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1512</v>
+      </c>
+      <c r="D10" s="11">
         <v>1</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6">
-        <f>E7*D7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="2">
+      <c r="E10" s="15">
+        <v>14.95</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="0"/>
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4">
+      <c r="C11" s="22">
+        <v>755</v>
+      </c>
+      <c r="D11" s="22">
         <v>1</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6">
-        <f>E8*D8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="2">
+      <c r="E11" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="24">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="19">
+        <v>70217642</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1</v>
+      </c>
+      <c r="E12" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="19">
+        <v>70063405</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1</v>
+      </c>
+      <c r="E13" s="15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="22">
+        <v>976</v>
+      </c>
+      <c r="D14" s="22">
+        <v>1</v>
+      </c>
+      <c r="E14" s="23">
+        <v>2.5</v>
+      </c>
+      <c r="F14" s="24">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="19">
+        <v>70100079</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="0"/>
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4">
+      <c r="B16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="14">
+        <v>70460944</v>
+      </c>
+      <c r="D16" s="11">
         <v>1</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6">
-        <f>E9*D9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="C10" s="8">
-        <v>1512</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="E16" s="15">
+        <v>6.95</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" si="0"/>
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="41">
+        <v>70460466</v>
+      </c>
+      <c r="D17" s="42">
         <v>1</v>
       </c>
-      <c r="E10" s="6">
-        <v>14.95</v>
-      </c>
-      <c r="F10" s="6">
-        <f>E10*D10</f>
-        <v>14.95</v>
-      </c>
-    </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4">
+      <c r="E17" s="43">
+        <v>1.5</v>
+      </c>
+      <c r="F17" s="44">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="26">
+        <v>70460903</v>
+      </c>
+      <c r="D18" s="26">
         <v>1</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6">
-        <f>E11*D11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6">
-        <f>E12*D12</f>
-        <v>0</v>
+      <c r="E18" s="27">
+        <v>4.5</v>
+      </c>
+      <c r="F18" s="28">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="37">
+        <f>SUM(F3:F10,F12:F13,F15:F18)</f>
+        <v>108.85500000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="38">
+        <f>F19*1.2</f>
+        <v>130.62600000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="39">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="C7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1547,94 +2177,140 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="9" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="9" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="9" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="9" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="9" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="9" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="256" width="8.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1">
+        <f>SUM(B1:B9)</f>
+        <v>6.75</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="46">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2">
+        <f>B11*50</f>
+        <v>400</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1642,94 +2318,89 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="10" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="10" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="10" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="10" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="10" customWidth="1"/>
+    <col min="1" max="256" width="8.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>